<commit_message>
Done with features #1 and #2
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thhllc-my.sharepoint.com/personal/bellian_otieno_griffinglobaltech_com/Documents/Documents/UiPath/Onboarding_Email_Coordinator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D70B673-38A1-48AB-A7B6-EFEE932D39AC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16470" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -159,7 +159,10 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>AutoRecrut</t>
+  </si>
+  <si>
+    <t>bello</t>
   </si>
 </sst>
 </file>
@@ -212,10 +215,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -537,16 +540,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -594,17 +597,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1623,12 +1628,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1670,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1681,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1795,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2782,14 +2787,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Populating queues with datafrom excel candidate summary
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\UiPath\HR_Internal\Onboarding_Email_Coordinator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9115EF-7BF6-48CE-B895-53B04B2EB49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -159,14 +159,20 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>CandidatesQueue</t>
+  </si>
+  <si>
+    <t>OnboardingEmailCoordinator</t>
+  </si>
+  <si>
+    <t>strExcelCandidatePath</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -190,6 +196,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -211,16 +222,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -239,9 +251,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +291,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +397,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -538,7 +550,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -598,7 +610,9 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
@@ -2782,7 +2796,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2828,7 +2844,17 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Issue#2 email handling (#8)
* Done with features #1 and #2

* stages

* Startups

* email handling

* Removed copies

* System Exceptions

* Changes

* Asset Fixes

* "Final changes"

* final commit
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thhllc-my.sharepoint.com/personal/bellian_otieno_griffinglobaltech_com/Documents/Documents/UiPath/Onboarding_Email_Coordinator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07741DBE-3F43-48C6-AB2F-6479FC173E5B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16470" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -159,7 +159,34 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>AutoRecrut</t>
+  </si>
+  <si>
+    <t>bello</t>
+  </si>
+  <si>
+    <t>BException_Email_Body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BException_Email_Subject </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SException_Email_Subject </t>
+  </si>
+  <si>
+    <t>SException_Email_Body</t>
+  </si>
+  <si>
+    <t>No Attachment Found</t>
+  </si>
+  <si>
+    <t>Hello , Kindly note that the Email provided had no attachment added on it ,Kind Regards Admin</t>
+  </si>
+  <si>
+    <t>Hi , Certain Errors were experienced In the system</t>
+  </si>
+  <si>
+    <t>System Error</t>
   </si>
 </sst>
 </file>
@@ -212,10 +239,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -236,6 +263,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -538,15 +569,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -594,17 +625,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1617,18 +1650,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1698,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1709,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1823,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1802,10 +1835,38 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2771,7 +2832,6 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2780,16 +2840,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="119.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2828,11 +2890,17 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" s="2"/>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2"/>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3822,11 +3890,6 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Issue#2 email handling (#8)"
This reverts commit 08e39c9b940feb8637e64015ea4f658aed2f49bc.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thhllc-my.sharepoint.com/personal/bellian_otieno_griffinglobaltech_com/Documents/Documents/UiPath/Onboarding_Email_Coordinator/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07741DBE-3F43-48C6-AB2F-6479FC173E5B}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16470" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -159,34 +159,7 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>AutoRecrut</t>
-  </si>
-  <si>
-    <t>bello</t>
-  </si>
-  <si>
-    <t>BException_Email_Body</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BException_Email_Subject </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SException_Email_Subject </t>
-  </si>
-  <si>
-    <t>SException_Email_Body</t>
-  </si>
-  <si>
-    <t>No Attachment Found</t>
-  </si>
-  <si>
-    <t>Hello , Kindly note that the Email provided had no attachment added on it ,Kind Regards Admin</t>
-  </si>
-  <si>
-    <t>Hi , Certain Errors were experienced In the system</t>
-  </si>
-  <si>
-    <t>System Error</t>
+    <t>ProcessABCQueue</t>
   </si>
 </sst>
 </file>
@@ -239,10 +212,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -263,10 +236,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -569,15 +538,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -625,19 +594,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1650,18 +1617,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z987"/>
+  <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1698,7 +1665,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1709,7 +1676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1823,7 +1790,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1835,38 +1802,10 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" t="s">
-        <v>53</v>
-      </c>
-    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2832,6 +2771,7 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
+    <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2840,18 +2780,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="119.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.36328125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2890,17 +2828,11 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2"/>
-    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="2"/>
-    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3890,6 +3822,11 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
+    <row r="996" ht="14.25" customHeight="1"/>
+    <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Feat : Mailing Handled
* Done with features #1 and #2

* stages

* Startups

* email handling

* Removed copies

* System Exceptions

* Changes

* Asset Fixes

* "Final changes"

* final commit
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thhllc-my.sharepoint.com/personal/bellian_otieno_griffinglobaltech_com/Documents/Documents/UiPath/Onboarding_Email_Coordinator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07741DBE-3F43-48C6-AB2F-6479FC173E5B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16470" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -159,7 +159,34 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>AutoRecrut</t>
+  </si>
+  <si>
+    <t>bello</t>
+  </si>
+  <si>
+    <t>BException_Email_Body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BException_Email_Subject </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SException_Email_Subject </t>
+  </si>
+  <si>
+    <t>SException_Email_Body</t>
+  </si>
+  <si>
+    <t>No Attachment Found</t>
+  </si>
+  <si>
+    <t>Hello , Kindly note that the Email provided had no attachment added on it ,Kind Regards Admin</t>
+  </si>
+  <si>
+    <t>Hi , Certain Errors were experienced In the system</t>
+  </si>
+  <si>
+    <t>System Error</t>
   </si>
 </sst>
 </file>
@@ -212,10 +239,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -236,6 +263,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -538,15 +569,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -594,17 +625,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1617,18 +1650,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1698,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1709,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1823,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1802,10 +1835,38 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2771,7 +2832,6 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2780,16 +2840,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="119.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2828,11 +2890,17 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" s="2"/>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2"/>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3822,11 +3890,6 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated sender email and BException email
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\UiPath\HR_Internal\Onboarding_Email_Coordinator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F933DB7-AD6B-45BB-B9BA-0E7AC8BF5654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096C8CBC-1D0C-4567-9E62-7F062BFFA6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16530" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -213,9 +213,6 @@
   </si>
   <si>
     <t>System Exception Error</t>
-  </si>
-  <si>
-    <t>str_BExceptionEmail</t>
   </si>
 </sst>
 </file>
@@ -1700,7 +1697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z985"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -2902,8 +2899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2983,12 +2980,8 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="A6" s="7"/>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Updated changes after demo
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\UiPath\HR_Internal\Onboarding_Email_Coordinator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096C8CBC-1D0C-4567-9E62-7F062BFFA6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3058E5A-0CB0-4E3E-BD4D-3BC9D9DE3249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16530" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>Hi, please ensure the Candidate Summary attachment is not empty.</t>
-  </si>
-  <si>
-    <t>Data\Exceptions</t>
   </si>
   <si>
     <t>Hi , I encountered an error during runtime.
@@ -213,6 +210,12 @@
   </si>
   <si>
     <t>System Exception Error</t>
+  </si>
+  <si>
+    <t>RobotAccountEmail</t>
+  </si>
+  <si>
+    <t>Exceptions_Screenshots\</t>
   </si>
 </sst>
 </file>
@@ -1697,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z985"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1771,7 +1774,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1901,7 +1904,7 @@
         <v>45</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
@@ -1909,7 +1912,7 @@
         <v>46</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
@@ -2899,8 +2902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2980,8 +2983,12 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="7"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
File deletion after addition to DB
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\UiPath\HR_Internal\Onboarding_Email_Coordinator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096C8CBC-1D0C-4567-9E62-7F062BFFA6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62ED45A1-847F-4FD6-8ADC-D5C5F1D25311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16530" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>Hi, please ensure the Candidate Summary attachment is not empty.</t>
-  </si>
-  <si>
-    <t>Data\Exceptions</t>
   </si>
   <si>
     <t>Hi , I encountered an error during runtime.
@@ -213,6 +210,12 @@
   </si>
   <si>
     <t>System Exception Error</t>
+  </si>
+  <si>
+    <t>RobotAccountEmail</t>
+  </si>
+  <si>
+    <t>Exceptions_Screenshots/</t>
   </si>
 </sst>
 </file>
@@ -1697,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z985"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1771,7 +1774,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1901,7 +1904,7 @@
         <v>45</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
@@ -1909,7 +1912,7 @@
         <v>46</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
@@ -2899,8 +2902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2980,8 +2983,12 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="7"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Extract email add queues (#20)
* Updated changes after demo

* Fixed .gitignore

* Fix - remove redundant sequences

---------

Co-authored-by: Fredrick Mutua <fredrick.mutua@griffinglobaltech.com>
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\UiPath\HR_Internal\Onboarding_Email_Coordinator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096C8CBC-1D0C-4567-9E62-7F062BFFA6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3791AB6-1129-42A7-8CE2-90E6EB517435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16530" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>Hi, please ensure the Candidate Summary attachment is not empty.</t>
-  </si>
-  <si>
-    <t>Data\Exceptions</t>
   </si>
   <si>
     <t>Hi , I encountered an error during runtime.
@@ -213,6 +210,12 @@
   </si>
   <si>
     <t>System Exception Error</t>
+  </si>
+  <si>
+    <t>RobotAccountEmail</t>
+  </si>
+  <si>
+    <t>Exceptions_Screenshots/</t>
   </si>
 </sst>
 </file>
@@ -1697,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z985"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1771,7 +1774,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1901,7 +1904,7 @@
         <v>45</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
@@ -1909,7 +1912,7 @@
         <v>46</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
@@ -2899,8 +2902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2980,8 +2983,12 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="7"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
File deletion after addition to DB (#21)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\UiPath\HR_Internal\Onboarding_Email_Coordinator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3791AB6-1129-42A7-8CE2-90E6EB517435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62ED45A1-847F-4FD6-8ADC-D5C5F1D25311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1701,7 +1701,7 @@
   <dimension ref="A1:Z985"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2903,7 +2903,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Exception recording and candidate DB population
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\UiPath\HR_Internal\Onboarding_Email_Coordinator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62ED45A1-847F-4FD6-8ADC-D5C5F1D25311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6772CDE-1460-4F4E-8E8A-5D84D8CBF504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -162,18 +162,9 @@
     <t xml:space="preserve">BException_Email_Subject </t>
   </si>
   <si>
-    <t xml:space="preserve">SException_Email_Subject </t>
-  </si>
-  <si>
     <t>SException_Email_Body</t>
   </si>
   <si>
-    <t>No Attachment Found</t>
-  </si>
-  <si>
-    <t>Hello , Kindly note that the Email provided had no attachment added on it ,Kind Regards Admin</t>
-  </si>
-  <si>
     <t>OnboardingProcessedFolder</t>
   </si>
   <si>
@@ -201,14 +192,6 @@
     <t>Empty excel attachment.</t>
   </si>
   <si>
-    <t>Hi, please ensure the Candidate Summary attachment is not empty.</t>
-  </si>
-  <si>
-    <t>Hi , I encountered an error during runtime.
-Source: @source
-Error: @error</t>
-  </si>
-  <si>
     <t>System Exception Error</t>
   </si>
   <si>
@@ -216,6 +199,57 @@
   </si>
   <si>
     <t>Exceptions_Screenshots/</t>
+  </si>
+  <si>
+    <t>No Attachment Found.</t>
+  </si>
+  <si>
+    <t>Hello, 
+Please note that the email sent had no Candidate Summary List attachment accompanying it.
+The Business exception has been recorded in the Reports Database's Exceptions table.
+Kind Regards,
+RPA Onboarding Bot (Dispatcher).</t>
+  </si>
+  <si>
+    <t>Hello, 
+Please ensure the Candidate Summary List attachment is not empty. 
+The exception has been recoreded in the Reports Database's Exceptions tables. 
+Kind Regards,
+RPA Onboarding Bot (Dispatcher).</t>
+  </si>
+  <si>
+    <t>Successful_Queue_and_DB_Population_Subject</t>
+  </si>
+  <si>
+    <t>Successful_Queue_and_DB_Population_Body</t>
+  </si>
+  <si>
+    <t>Successful population of Queue and Database</t>
+  </si>
+  <si>
+    <t>Hi,
+Job complete. @rows candidates have been added to the Orchestrator Queue  affecting @db_rows rows in the database.
+Regards,
+RPA Onboarding Bot (Dispatcher).</t>
+  </si>
+  <si>
+    <t>InsertCandididatestoDBCommand</t>
+  </si>
+  <si>
+    <t>InsertSExceptiontoDBCommand</t>
+  </si>
+  <si>
+    <t>SException_Email_Subject</t>
+  </si>
+  <si>
+    <t>Hello, 
+A System Exception occurred during runtime. The error has been recorded in the Reports Database's Exceptions table.
+Exception source: @source
+Exception message: @error
+Affected Row Count: @int_affectedRowCount
+Please find a screenshot of the same is attached below.
+Kind Regards,
+RPA Onboarding Bot (Dispatcher).</t>
   </si>
 </sst>
 </file>
@@ -285,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -299,6 +333,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -667,7 +704,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -678,7 +715,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -1698,10 +1735,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z985"/>
+  <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1774,7 +1811,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1882,34 +1919,36 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.4">
+      <c r="C18" s="3"/>
+    </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>48</v>
+      <c r="A19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>60</v>
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>59</v>
@@ -1917,24 +1956,44 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" customHeight="1">
+      <c r="A27" s="2"/>
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+    </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2892,6 +2951,9 @@
     <row r="983" ht="14.25" customHeight="1"/>
     <row r="984" ht="14.25" customHeight="1"/>
     <row r="985" ht="14.25" customHeight="1"/>
+    <row r="986" ht="14.25" customHeight="1"/>
+    <row r="987" ht="14.25" customHeight="1"/>
+    <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2902,8 +2964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2952,46 +3014,60 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>